<commit_message>
FIX: [FULLSTACK] Some Task (#90)
* FIX: [FULLSTACK] Some Task

- Fix Empty data conditions on the Vehicle Excel feature
- Fix Pagination Bug on Admin panel
- Fix the Phone number when creating a payment request
- Change Vehicle use from agency to commercial
- Remove unused variable
- Remove mandatory from vehicle_type_code
- Fix Admin Panel still showing when 404
</commit_message>
<xml_diff>
--- a/core-admin/view/static/doc/Tokopolis Vehicle Data.xlsx
+++ b/core-admin/view/static/doc/Tokopolis Vehicle Data.xlsx
@@ -43,7 +43,10 @@
     <t>Vehicle Category Code</t>
   </si>
   <si>
-    <t>Vehicle Function</t>
+    <t>Vehicle Function (Private)</t>
+  </si>
+  <si>
+    <t>Vehicle Function (Commercial)</t>
   </si>
   <si>
     <t>Comprehensive Coverage</t>
@@ -52,7 +55,7 @@
     <t>TLO Coverage</t>
   </si>
   <si>
-    <t>Hatchback, Minibus, Sedan</t>
+    <t>Hatchback, Minibus, Sedan, etc</t>
   </si>
   <si>
     <t>VT000X</t>
@@ -64,10 +67,7 @@
     <t>A or C</t>
   </si>
   <si>
-    <t>1 - Private, 0 - Dinas</t>
-  </si>
-  <si>
-    <t>1 - Commercial</t>
+    <t>1 - Supported, 0 - Not Supported</t>
   </si>
   <si>
     <t>1 - Comprehensive, 0 - Not Supported</t>
@@ -81,10 +81,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -98,13 +98,15 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="&quot;Times New Roman&quot;"/>
+      <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -122,10 +124,132 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -138,142 +262,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,187 +290,199 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.8"/>
+        <bgColor rgb="FFFFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -581,6 +595,62 @@
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,6 +660,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -611,226 +690,161 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -860,6 +874,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1124,23 +1142,23 @@
   <dimension ref="A1:AC12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="$A3:$XFD3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.75" customWidth="1"/>
-    <col min="2" max="2" width="16.1339285714286" customWidth="1"/>
-    <col min="3" max="3" width="14.25" customWidth="1"/>
-    <col min="4" max="4" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="20.5357142857143" customWidth="1"/>
+    <col min="2" max="2" width="16.6696428571429" customWidth="1"/>
+    <col min="3" max="3" width="17.1071428571429" customWidth="1"/>
+    <col min="4" max="4" width="17.4017857142857" customWidth="1"/>
     <col min="5" max="5" width="47.6339285714286" customWidth="1"/>
     <col min="6" max="6" width="36.3839285714286" customWidth="1"/>
     <col min="7" max="7" width="21.8839285714286" customWidth="1"/>
     <col min="8" max="8" width="27.5" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
-    <col min="10" max="10" width="26.3839285714286" customWidth="1"/>
-    <col min="11" max="11" width="16.8839285714286" customWidth="1"/>
-    <col min="12" max="12" width="25.6339285714286" customWidth="1"/>
+    <col min="10" max="10" width="30.3571428571429" customWidth="1"/>
+    <col min="11" max="11" width="34.5267857142857" customWidth="1"/>
+    <col min="12" max="12" width="29.6160714285714" customWidth="1"/>
     <col min="13" max="13" width="23.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1176,83 +1194,83 @@
         <v>9</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2">
+        <v>12</v>
+      </c>
+      <c r="N1" s="13">
         <v>2022</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="13">
         <v>2021</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="13">
         <v>2020</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="13">
         <v>2019</v>
       </c>
-      <c r="R1" s="2">
+      <c r="R1" s="13">
         <v>2018</v>
       </c>
-      <c r="S1" s="2">
+      <c r="S1" s="13">
         <v>2017</v>
       </c>
-      <c r="T1" s="2">
+      <c r="T1" s="13">
         <v>2016</v>
       </c>
-      <c r="U1" s="2">
+      <c r="U1" s="13">
         <v>2015</v>
       </c>
-      <c r="V1" s="2">
+      <c r="V1" s="13">
         <v>2014</v>
       </c>
-      <c r="W1" s="2">
+      <c r="W1" s="13">
         <v>2013</v>
       </c>
-      <c r="X1" s="2">
+      <c r="X1" s="13">
         <v>2012</v>
       </c>
-      <c r="Y1" s="2">
+      <c r="Y1" s="13">
         <v>2011</v>
       </c>
-      <c r="Z1" s="2">
+      <c r="Z1" s="13">
         <v>2010</v>
       </c>
-      <c r="AA1" s="2">
+      <c r="AA1" s="13">
         <v>2009</v>
       </c>
-      <c r="AB1" s="2">
+      <c r="AB1" s="13">
         <v>2008</v>
       </c>
-      <c r="AC1" s="2">
+      <c r="AC1" s="13">
         <v>2007</v>
       </c>
     </row>
-    <row r="2" ht="12" spans="1:29">
+    <row r="2" spans="1:29">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>17</v>
@@ -1263,22 +1281,22 @@
       <c r="M2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="5"/>

</xml_diff>